<commit_message>
Update with Boutprocess bug fix
</commit_message>
<xml_diff>
--- a/helperfiles/Prey_Key_Comments.xlsx
+++ b/helperfiles/Prey_Key_Comments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/helperfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{479E058C-EDFC-4B08-996F-0C0FEAA1A8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11DCFE25-5DDB-4B31-AE02-B4BE39C62932}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{479E058C-EDFC-4B08-996F-0C0FEAA1A8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC657509-4D2F-4F46-B876-DE37176DB0D8}"/>
   <bookViews>
-    <workbookView xWindow="30495" yWindow="1170" windowWidth="24150" windowHeight="14760" xr2:uid="{8A50F331-599A-4FF6-9C19-63B062338315}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38805" windowHeight="18315" xr2:uid="{8A50F331-599A-4FF6-9C19-63B062338315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Comment</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Enter a list of mutually exclusive prey types for analysis, with a unique 3 or 4 letter code for each. You should limit the number of possible prey types such that each type is represented by a reasonable number of instances in the data set (see "N" nolumn in previous worksheet: a minimum of 25 is a good rule of thumb, at least 50 preferred).  Thus prey codes with few observations should be combined into a single prey type.  NOTE: The FIRST row is reserved for the "UNID" prey type (un-identified prey): leave this as-is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If desired, enter minimum size (mm) for items of this prey type </t>
   </si>
 </sst>
 </file>
@@ -125,9 +128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -165,7 +168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -271,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -413,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D70958F-E336-4A0B-A12D-8F8727A902F9}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +521,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>